<commit_message>
Add Info to Philadelphia (9)
</commit_message>
<xml_diff>
--- a/Treatment components.xlsx
+++ b/Treatment components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bened\Desktop\treatment-components-website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bened\Desktop\Projekte\GitHub\peds-iipt-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA1AFD2-077C-4116-B7F3-427B0703BE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C133115-A0C4-401E-AAE9-08A10842F6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5E5E90C4-9D26-40A7-8F5F-F1D264C7327F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{5E5E90C4-9D26-40A7-8F5F-F1D264C7327F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -575,7 +575,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1290,7 +1290,7 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -1334,7 +1334,7 @@
         <v>1</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1378,7 +1378,7 @@
         <v>1</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1466,7 +1466,7 @@
         <v>1</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -1510,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -1554,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -1733,7 +1733,7 @@
         <v>1</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -1777,7 +1777,7 @@
         <v>1</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -2264,7 +2264,7 @@
         <v>1</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38">
         <v>0</v>
@@ -2352,7 +2352,7 @@
         <v>1</v>
       </c>
       <c r="K40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L40">
         <v>0</v>
@@ -2396,7 +2396,7 @@
         <v>1</v>
       </c>
       <c r="K41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41">
         <v>0</v>

</xml_diff>

<commit_message>
Add info to Calgary (12)
</commit_message>
<xml_diff>
--- a/Treatment components.xlsx
+++ b/Treatment components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bened\Desktop\Projekte\GitHub\peds-iipt-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C133115-A0C4-401E-AAE9-08A10842F6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845A3BB5-EB73-4CD2-B269-28DB87162FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{5E5E90C4-9D26-40A7-8F5F-F1D264C7327F}"/>
   </bookViews>
@@ -575,7 +575,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -1029,7 +1029,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1563,7 +1563,7 @@
         <v>1</v>
       </c>
       <c r="N22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1607,7 +1607,7 @@
         <v>0</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1654,7 +1654,7 @@
         <v>1</v>
       </c>
       <c r="N24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24">
         <v>1</v>
@@ -2053,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="N33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O33">
         <v>0</v>
@@ -2185,7 +2185,7 @@
         <v>1</v>
       </c>
       <c r="N36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -2229,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="N37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O37">
         <v>0</v>
@@ -2273,7 +2273,7 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O38">
         <v>0</v>
@@ -2405,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="N41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O41">
         <v>0</v>

</xml_diff>

<commit_message>
Add info to Cincinnati (10)
</commit_message>
<xml_diff>
--- a/Treatment components.xlsx
+++ b/Treatment components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bened\Desktop\Projekte\GitHub\peds-iipt-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845A3BB5-EB73-4CD2-B269-28DB87162FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19B3B80-9EEC-475F-AFD5-AA886DF51A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{5E5E90C4-9D26-40A7-8F5F-F1D264C7327F}"/>
   </bookViews>
@@ -575,7 +575,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -753,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -1114,7 +1114,7 @@
         <v>1</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -1249,7 +1249,7 @@
         <v>1</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -1337,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -1381,7 +1381,7 @@
         <v>1</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -1469,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -1513,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -1557,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -1692,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -1736,7 +1736,7 @@
         <v>1</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -1780,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -2003,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="L37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37">
         <v>0</v>
@@ -2267,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="L38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38">
         <v>0</v>

</xml_diff>